<commit_message>
edited in some Args in Init ALL APPs
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>15933527amam</t>
+  </si>
+  <si>
+    <t>ACME_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/</t>
   </si>
 </sst>
 </file>
@@ -514,7 +520,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -599,7 +605,14 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1592,6 +1605,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
edit some fuckin args
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -176,9 +176,6 @@
     <t>ACME_Password</t>
   </si>
   <si>
-    <t>amagdy529@gmail.com</t>
-  </si>
-  <si>
     <t>15933527amam</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>amagdy529XS@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -602,15 +602,15 @@
         <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>